<commit_message>
site update following final data collection session
</commit_message>
<xml_diff>
--- a/data/GOZO_assignment_count.xlsx
+++ b/data/GOZO_assignment_count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B630C660-63DA-EA43-B244-3FDB48EFAE97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8E11E1-2DED-EB46-A537-3CDBEE95A576}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="3200" windowWidth="28800" windowHeight="16160" xr2:uid="{2FF04964-7F32-AF41-A5F9-FFB2D5CCFF2D}"/>
+    <workbookView xWindow="39660" yWindow="3820" windowWidth="28800" windowHeight="16160" xr2:uid="{2FF04964-7F32-AF41-A5F9-FFB2D5CCFF2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5B556-9057-0343-A18D-6714DE7E2CA0}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,6 +562,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>